<commit_message>
logboekupdate , presentatie , infoactivity
</commit_message>
<xml_diff>
--- a/Drive/Logboeken/Logboek Daniël Lin.xlsx
+++ b/Drive/Logboeken/Logboek Daniël Lin.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
   <si>
     <t>Datum</t>
   </si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t>Werken aan interface</t>
+  </si>
+  <si>
+    <t>online meeting, betere taakverdeling, en wekelijkse resultaten</t>
+  </si>
+  <si>
+    <t>Kleine powerpoint, infoactivity afmaken</t>
   </si>
 </sst>
 </file>
@@ -452,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -503,11 +509,11 @@
       </c>
       <c r="F2">
         <f>SUM(D:D)</f>
-        <v>37.5</v>
+        <v>39</v>
       </c>
       <c r="G2">
         <f>SUM(210,-F2)</f>
-        <v>172.5</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -774,6 +780,34 @@
       </c>
       <c r="D21" s="4">
         <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
+        <v>42352</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
+        <v>42352</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="4">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
kleine setup selectionActivity en EindschermActivity
</commit_message>
<xml_diff>
--- a/Drive/Logboeken/Logboek Daniël Lin.xlsx
+++ b/Drive/Logboeken/Logboek Daniël Lin.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="42">
   <si>
     <t>Datum</t>
   </si>
@@ -129,7 +129,22 @@
     <t>Kleine powerpoint maken, infoactivity afmaken</t>
   </si>
   <si>
-    <t>presentatie voorbereiden</t>
+    <t>presentatie voorbereiden, powerpoint uitbreiden</t>
+  </si>
+  <si>
+    <t>laatste voorbereiding presentatie</t>
+  </si>
+  <si>
+    <t>tussenpresentatie</t>
+  </si>
+  <si>
+    <t>projectdocument bijwerken</t>
+  </si>
+  <si>
+    <t>gebruikshandleiding maken</t>
+  </si>
+  <si>
+    <t>Globale opzet eindschermActivity en selectionActivity</t>
   </si>
 </sst>
 </file>
@@ -461,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -512,11 +527,11 @@
       </c>
       <c r="F2">
         <f>SUM(D:D)</f>
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="G2">
         <f>SUM(210,-F2)</f>
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -824,6 +839,76 @@
         <v>36</v>
       </c>
       <c r="D24" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="6">
+        <v>42354</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
+        <v>42354</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="6">
+        <v>42356</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="6">
+        <v>42359</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="6">
+        <v>42359</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D29" s="4">
         <v>1</v>
       </c>
     </row>

</xml_diff>